<commit_message>
back up some experimental results
</commit_message>
<xml_diff>
--- a/evaluation/lemmas/results.xlsx
+++ b/evaluation/lemmas/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="35">
   <si>
     <t xml:space="preserve">structural</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">checksum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f(...g(...)) = ?</t>
   </si>
   <si>
     <t xml:space="preserve">Z3 hangs on push</t>
@@ -224,7 +221,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,6 +247,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -458,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W35" activeCellId="0" sqref="W35:W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,7 +566,7 @@
       <c r="G4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="5" t="n">
@@ -1030,7 +1031,7 @@
       <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="5" t="n">
         <v>30</v>
       </c>
@@ -1658,7 +1659,7 @@
       <c r="G28" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="H28" s="7"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="5" t="n">
         <v>30</v>
       </c>
@@ -1993,9 +1994,7 @@
         <f aca="false">I36/$C36</f>
         <v>0</v>
       </c>
-      <c r="W36" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="W36" s="5"/>
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
@@ -2307,16 +2306,16 @@
       <c r="I42" s="5" t="n">
         <v>136</v>
       </c>
-      <c r="J42" s="8" t="n">
+      <c r="J42" s="9" t="n">
         <v>0.437199074074074</v>
       </c>
-      <c r="K42" s="8" t="n">
+      <c r="K42" s="9" t="n">
         <v>0.445706018518519</v>
       </c>
-      <c r="L42" s="8" t="n">
+      <c r="L42" s="9" t="n">
         <v>0.44806712962963</v>
       </c>
-      <c r="M42" s="9" t="n">
+      <c r="M42" s="10" t="n">
         <f aca="false">L42-J42</f>
         <v>0.0108680555555556</v>
       </c>
@@ -2366,13 +2365,13 @@
         <v>20</v>
       </c>
       <c r="B43" s="5"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
       <c r="P43" s="1" t="e">
         <f aca="false">D43/$C43</f>
         <v>#DIV/0!</v>
@@ -2416,7 +2415,7 @@
         <v>21</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G44" s="5" t="n">
         <v>14</v>
@@ -2511,10 +2510,10 @@
       </c>
       <c r="L48" s="5"/>
       <c r="M48" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N48" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="N48" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="P48" s="1" t="s">
         <v>4</v>
@@ -2561,18 +2560,18 @@
       <c r="I49" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J49" s="10" t="n">
+      <c r="J49" s="11" t="n">
         <v>0.313888888888889</v>
       </c>
-      <c r="K49" s="10" t="n">
+      <c r="K49" s="11" t="n">
         <v>0.31431712962963</v>
       </c>
-      <c r="L49" s="10"/>
-      <c r="M49" s="9" t="n">
+      <c r="L49" s="11"/>
+      <c r="M49" s="10" t="n">
         <f aca="false">K49-J49</f>
         <v>0.000428240740740741</v>
       </c>
-      <c r="N49" s="9"/>
+      <c r="N49" s="10"/>
       <c r="P49" s="1" t="n">
         <f aca="false">D49/$C49</f>
         <v>1</v>
@@ -2624,14 +2623,14 @@
       <c r="I50" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="J50" s="10" t="n">
+      <c r="J50" s="11" t="n">
         <v>0.314525462962963</v>
       </c>
-      <c r="K50" s="10" t="n">
+      <c r="K50" s="11" t="n">
         <v>0.314560185185185</v>
       </c>
-      <c r="L50" s="10"/>
-      <c r="M50" s="9" t="n">
+      <c r="L50" s="11"/>
+      <c r="M50" s="10" t="n">
         <f aca="false">K50-J50</f>
         <v>3.47222222222222E-005</v>
       </c>
@@ -2686,14 +2685,14 @@
       <c r="I51" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="J51" s="10" t="n">
+      <c r="J51" s="11" t="n">
         <v>0.314583333333333</v>
       </c>
-      <c r="K51" s="10" t="n">
+      <c r="K51" s="11" t="n">
         <v>0.314583333333333</v>
       </c>
-      <c r="L51" s="10"/>
-      <c r="M51" s="9" t="n">
+      <c r="L51" s="11"/>
+      <c r="M51" s="10" t="n">
         <f aca="false">K51-J51</f>
         <v>0</v>
       </c>
@@ -2739,28 +2738,28 @@
       <c r="F52" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G52" s="11" t="n">
+      <c r="G52" s="12" t="n">
         <v>26</v>
       </c>
-      <c r="H52" s="11" t="n">
+      <c r="H52" s="12" t="n">
         <v>30</v>
       </c>
       <c r="I52" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="J52" s="10" t="n">
+      <c r="J52" s="11" t="n">
         <v>0.391168981481482</v>
       </c>
-      <c r="K52" s="10" t="n">
+      <c r="K52" s="11" t="n">
         <v>0.400787037037037</v>
       </c>
-      <c r="L52" s="10"/>
-      <c r="M52" s="9" t="n">
+      <c r="L52" s="11"/>
+      <c r="M52" s="10" t="n">
         <f aca="false">K52-J52</f>
         <v>0.00961805555555556</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P52" s="1" t="n">
         <f aca="false">D52/$C52</f>
@@ -2813,18 +2812,18 @@
       <c r="I53" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="J53" s="10" t="n">
+      <c r="J53" s="11" t="n">
         <v>0.326851851851852</v>
       </c>
-      <c r="K53" s="10" t="n">
+      <c r="K53" s="11" t="n">
         <v>0.336446759259259</v>
       </c>
-      <c r="L53" s="10"/>
-      <c r="M53" s="9" t="n">
+      <c r="L53" s="11"/>
+      <c r="M53" s="10" t="n">
         <f aca="false">K53-J53</f>
         <v>0.00959490740740741</v>
       </c>
-      <c r="N53" s="10" t="n">
+      <c r="N53" s="11" t="n">
         <v>0.439861111111111</v>
       </c>
       <c r="P53" s="1" t="n">
@@ -2878,14 +2877,14 @@
       <c r="I54" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="J54" s="10" t="n">
+      <c r="J54" s="11" t="n">
         <v>0.476678240740741</v>
       </c>
-      <c r="K54" s="10" t="n">
+      <c r="K54" s="11" t="n">
         <v>0.476701388888889</v>
       </c>
-      <c r="L54" s="10"/>
-      <c r="M54" s="9" t="n">
+      <c r="L54" s="11"/>
+      <c r="M54" s="10" t="n">
         <f aca="false">K54-J54</f>
         <v>2.31481481481481E-005</v>
       </c>
@@ -2940,14 +2939,14 @@
       <c r="I55" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="J55" s="10" t="n">
+      <c r="J55" s="11" t="n">
         <v>0.476840277777778</v>
       </c>
-      <c r="K55" s="10" t="n">
+      <c r="K55" s="11" t="n">
         <v>0.478958333333333</v>
       </c>
-      <c r="L55" s="10"/>
-      <c r="M55" s="9" t="n">
+      <c r="L55" s="11"/>
+      <c r="M55" s="10" t="n">
         <f aca="false">K55-J55</f>
         <v>0.00211805555555556</v>
       </c>
@@ -3002,14 +3001,14 @@
       <c r="I56" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="J56" s="10" t="n">
+      <c r="J56" s="11" t="n">
         <v>0.390173611111111</v>
       </c>
-      <c r="K56" s="10" t="n">
+      <c r="K56" s="11" t="n">
         <v>0.39037037037037</v>
       </c>
-      <c r="L56" s="10"/>
-      <c r="M56" s="9" t="n">
+      <c r="L56" s="11"/>
+      <c r="M56" s="10" t="n">
         <f aca="false">K56-J56</f>
         <v>0.000196759259259259</v>
       </c>
@@ -3050,11 +3049,11 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
-      <c r="J57" s="10"/>
-      <c r="K57" s="10"/>
-      <c r="L57" s="10"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="10"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="11"/>
       <c r="P57" s="1" t="e">
         <f aca="false">D57/$C57</f>
         <v>#DIV/0!</v>
@@ -3103,19 +3102,19 @@
       <c r="H58" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="I58" s="7"/>
-      <c r="J58" s="10" t="n">
+      <c r="I58" s="8"/>
+      <c r="J58" s="11" t="n">
         <v>0.459027777777778</v>
       </c>
-      <c r="K58" s="10" t="n">
+      <c r="K58" s="11" t="n">
         <v>0.459027777777778</v>
       </c>
-      <c r="L58" s="10"/>
-      <c r="M58" s="9" t="n">
+      <c r="L58" s="11"/>
+      <c r="M58" s="10" t="n">
         <f aca="false">K58-J58</f>
         <v>0</v>
       </c>
-      <c r="N58" s="10" t="n">
+      <c r="N58" s="11" t="n">
         <v>0.570798611111111</v>
       </c>
       <c r="P58" s="1" t="n">
@@ -3163,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P59" s="1" t="n">
         <f aca="false">D59/$C59</f>

</xml_diff>

<commit_message>
update lots of results
</commit_message>
<xml_diff>
--- a/evaluation/lemmas/results.xlsx
+++ b/evaluation/lemmas/results.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="first experiments" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="paper" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="second experiments" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="timing" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="69">
   <si>
     <t xml:space="preserve">structural</t>
   </si>
@@ -166,22 +167,87 @@
   <si>
     <t xml:space="preserve">evaluation/lemmas/tree.structural.bpl</t>
   </si>
+  <si>
+    <t xml:space="preserve">round 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">round 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">round 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time round 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time round 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time round 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last reported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">killed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productive time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">running time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map (sm06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove (sm06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate (sm06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">runlength (sm06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nat (sm06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">killed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list (sm06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tree (sm06)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="[hh]:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="[hh]:mm:ss.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -203,9 +269,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +306,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF579D1C"/>
       </patternFill>
     </fill>
   </fills>
@@ -265,7 +349,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,15 +378,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -310,15 +390,63 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -375,7 +503,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
@@ -410,7 +538,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$66</c:f>
+              <c:f>'second experiments'!$A$66</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -435,11 +563,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -455,7 +587,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$65:$E$65</c:f>
+              <c:f>'second experiments'!$B$65:$E$65</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -475,7 +607,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$66:$E$66</c:f>
+              <c:f>'second experiments'!$B$66:$E$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -500,7 +632,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$67</c:f>
+              <c:f>'second experiments'!$A$67</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -525,11 +657,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -545,7 +681,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$65:$E$65</c:f>
+              <c:f>'second experiments'!$B$65:$E$65</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -565,7 +701,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$67:$E$67</c:f>
+              <c:f>'second experiments'!$B$67:$E$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -590,7 +726,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$68</c:f>
+              <c:f>'second experiments'!$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -615,11 +751,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -635,7 +775,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$65:$E$65</c:f>
+              <c:f>'second experiments'!$B$65:$E$65</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -655,7 +795,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$68:$E$68</c:f>
+              <c:f>'second experiments'!$B$68:$E$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -680,7 +820,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$69</c:f>
+              <c:f>'second experiments'!$A$69</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -705,11 +845,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -725,7 +869,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$65:$E$65</c:f>
+              <c:f>'second experiments'!$B$65:$E$65</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -745,7 +889,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$69:$E$69</c:f>
+              <c:f>'second experiments'!$B$69:$E$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -770,7 +914,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$70</c:f>
+              <c:f>'second experiments'!$A$70</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -795,11 +939,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -815,7 +963,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$65:$E$65</c:f>
+              <c:f>'second experiments'!$B$65:$E$65</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -835,7 +983,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$70:$E$70</c:f>
+              <c:f>'second experiments'!$B$70:$E$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -860,7 +1008,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$71</c:f>
+              <c:f>'second experiments'!$A$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -885,11 +1033,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -905,7 +1057,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$65:$E$65</c:f>
+              <c:f>'second experiments'!$B$65:$E$65</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -925,7 +1077,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$71:$E$71</c:f>
+              <c:f>'second experiments'!$B$71:$E$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -947,17 +1099,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="67675618"/>
-        <c:axId val="43990847"/>
+        <c:axId val="47054592"/>
+        <c:axId val="96785300"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67675618"/>
+        <c:axId val="47054592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -974,12 +1126,15 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43990847"/>
+        <c:crossAx val="96785300"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -987,7 +1142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43990847"/>
+        <c:axId val="96785300"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1157,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1019,12 +1174,15 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67675618"/>
+        <c:crossAx val="47054592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1052,6 +1210,9 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
@@ -1088,7 +1249,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$74</c:f>
+              <c:f>'second experiments'!$A$74</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1113,11 +1274,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1133,7 +1298,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$73:$E$73</c:f>
+              <c:f>'second experiments'!$B$73:$E$73</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1153,7 +1318,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$74:$E$74</c:f>
+              <c:f>'second experiments'!$B$74:$E$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1178,7 +1343,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$75</c:f>
+              <c:f>'second experiments'!$A$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1203,11 +1368,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1223,7 +1392,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$73:$E$73</c:f>
+              <c:f>'second experiments'!$B$73:$E$73</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1243,7 +1412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$75:$E$75</c:f>
+              <c:f>'second experiments'!$B$75:$E$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1268,7 +1437,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$76</c:f>
+              <c:f>'second experiments'!$A$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1293,11 +1462,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1313,7 +1486,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$73:$E$73</c:f>
+              <c:f>'second experiments'!$B$73:$E$73</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1333,7 +1506,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$76:$E$76</c:f>
+              <c:f>'second experiments'!$B$76:$E$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1358,7 +1531,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$77</c:f>
+              <c:f>'second experiments'!$A$77</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1383,11 +1556,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1403,7 +1580,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$73:$E$73</c:f>
+              <c:f>'second experiments'!$B$73:$E$73</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1423,7 +1600,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$77:$E$77</c:f>
+              <c:f>'second experiments'!$B$77:$E$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1448,7 +1625,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$78</c:f>
+              <c:f>'second experiments'!$A$78</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1473,11 +1650,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1493,7 +1674,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$73:$E$73</c:f>
+              <c:f>'second experiments'!$B$73:$E$73</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1513,7 +1694,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$78:$E$78</c:f>
+              <c:f>'second experiments'!$B$78:$E$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1538,7 +1719,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$79</c:f>
+              <c:f>'second experiments'!$A$79</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1563,11 +1744,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1583,7 +1768,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$73:$E$73</c:f>
+              <c:f>'second experiments'!$B$73:$E$73</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1603,7 +1788,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$79:$E$79</c:f>
+              <c:f>'second experiments'!$B$79:$E$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1625,17 +1810,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="42703755"/>
-        <c:axId val="32793946"/>
+        <c:axId val="26364776"/>
+        <c:axId val="67957644"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42703755"/>
+        <c:axId val="26364776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1652,12 +1837,15 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32793946"/>
+        <c:crossAx val="67957644"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1665,7 +1853,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32793946"/>
+        <c:axId val="67957644"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,7 +1868,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1697,12 +1885,15 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42703755"/>
+        <c:crossAx val="26364776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1730,6 +1921,9 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
@@ -1766,7 +1960,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$82</c:f>
+              <c:f>'second experiments'!$A$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1791,11 +1985,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1811,7 +2009,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$81:$E$81</c:f>
+              <c:f>'second experiments'!$B$81:$E$81</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1831,7 +2029,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$82:$E$82</c:f>
+              <c:f>'second experiments'!$B$82:$E$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1856,7 +2054,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$83</c:f>
+              <c:f>'second experiments'!$A$83</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1881,11 +2079,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1901,7 +2103,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$81:$E$81</c:f>
+              <c:f>'second experiments'!$B$81:$E$81</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1921,7 +2123,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$83:$E$83</c:f>
+              <c:f>'second experiments'!$B$83:$E$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1946,7 +2148,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$84</c:f>
+              <c:f>'second experiments'!$A$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1971,11 +2173,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1991,7 +2197,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$81:$E$81</c:f>
+              <c:f>'second experiments'!$B$81:$E$81</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2011,7 +2217,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$84:$E$84</c:f>
+              <c:f>'second experiments'!$B$84:$E$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2036,7 +2242,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$85</c:f>
+              <c:f>'second experiments'!$A$85</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2061,11 +2267,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2081,7 +2291,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$81:$E$81</c:f>
+              <c:f>'second experiments'!$B$81:$E$81</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2101,7 +2311,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$85:$E$85</c:f>
+              <c:f>'second experiments'!$B$85:$E$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2126,7 +2336,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$86</c:f>
+              <c:f>'second experiments'!$A$86</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2151,11 +2361,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2171,7 +2385,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$81:$E$81</c:f>
+              <c:f>'second experiments'!$B$81:$E$81</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2191,7 +2405,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$86:$E$86</c:f>
+              <c:f>'second experiments'!$B$86:$E$86</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2216,7 +2430,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>paper!$A$87</c:f>
+              <c:f>'second experiments'!$A$87</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2241,11 +2455,15 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2261,7 +2479,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>paper!$B$81:$E$81</c:f>
+              <c:f>'second experiments'!$B$81:$E$81</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2281,7 +2499,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>paper!$B$87:$E$87</c:f>
+              <c:f>'second experiments'!$B$87:$E$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2303,17 +2521,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="36261422"/>
-        <c:axId val="43045928"/>
+        <c:axId val="1106689"/>
+        <c:axId val="63928896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="36261422"/>
+        <c:axId val="1106689"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2330,12 +2548,15 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43045928"/>
+        <c:crossAx val="63928896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2343,7 +2564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43045928"/>
+        <c:axId val="63928896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2358,7 +2579,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2375,12 +2596,15 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36261422"/>
+        <c:crossAx val="1106689"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2408,6 +2632,9 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
@@ -2439,9 +2666,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>456480</xdr:colOff>
+      <xdr:colOff>455400</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2450,7 +2677,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5263920" y="4790160"/>
-        <a:ext cx="5758920" cy="3241440"/>
+        <a:ext cx="5757840" cy="3240360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2469,9 +2696,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>515520</xdr:colOff>
+      <xdr:colOff>514440</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2480,7 +2707,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11825280" y="6999480"/>
-        <a:ext cx="5758920" cy="3241800"/>
+        <a:ext cx="5757840" cy="3240720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2499,9 +2726,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>99000</xdr:colOff>
+      <xdr:colOff>97920</xdr:colOff>
       <xdr:row>85</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2510,7 +2737,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4906440" y="10585440"/>
-        <a:ext cx="5758920" cy="3241440"/>
+        <a:ext cx="5757840" cy="3240360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2636,8 +2863,8 @@
   </sheetPr>
   <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2675,7 +2902,7 @@
       <c r="U2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -2743,7 +2970,7 @@
       <c r="G4" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="H4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="5" t="n">
@@ -3208,7 +3435,7 @@
       <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="5" t="n">
         <v>30</v>
       </c>
@@ -3256,7 +3483,7 @@
       <c r="H14" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="5" t="n">
         <v>8</v>
       </c>
       <c r="P14" s="1" t="n">
@@ -3836,7 +4063,7 @@
       <c r="G28" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="H28" s="8"/>
+      <c r="H28" s="7"/>
       <c r="I28" s="5" t="n">
         <v>30</v>
       </c>
@@ -3884,7 +4111,7 @@
       <c r="H29" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I29" s="0" t="n">
+      <c r="I29" s="5" t="n">
         <v>8</v>
       </c>
       <c r="P29" s="1" t="n">
@@ -4483,16 +4710,16 @@
       <c r="I42" s="5" t="n">
         <v>136</v>
       </c>
-      <c r="J42" s="9" t="n">
+      <c r="J42" s="8" t="n">
         <v>0.437199074074074</v>
       </c>
-      <c r="K42" s="9" t="n">
+      <c r="K42" s="8" t="n">
         <v>0.445706018518519</v>
       </c>
-      <c r="L42" s="9" t="n">
+      <c r="L42" s="8" t="n">
         <v>0.44806712962963</v>
       </c>
-      <c r="M42" s="10" t="n">
+      <c r="M42" s="9" t="n">
         <f aca="false">L42-J42</f>
         <v>0.0108680555555556</v>
       </c>
@@ -4542,13 +4769,13 @@
         <v>20</v>
       </c>
       <c r="B43" s="5"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
       <c r="P43" s="1" t="e">
         <f aca="false">D43/$C43</f>
         <v>#DIV/0!</v>
@@ -4573,7 +4800,7 @@
         <f aca="false">I43/$C43</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W43" s="0" t="n">
+      <c r="W43" s="5" t="n">
         <v>320978</v>
       </c>
     </row>
@@ -4737,18 +4964,18 @@
       <c r="I49" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J49" s="11" t="n">
+      <c r="J49" s="8" t="n">
         <v>0.313888888888889</v>
       </c>
-      <c r="K49" s="11" t="n">
+      <c r="K49" s="8" t="n">
         <v>0.31431712962963</v>
       </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="10" t="n">
+      <c r="L49" s="8"/>
+      <c r="M49" s="9" t="n">
         <f aca="false">K49-J49</f>
         <v>0.000428240740740741</v>
       </c>
-      <c r="N49" s="10"/>
+      <c r="N49" s="9"/>
       <c r="P49" s="1" t="n">
         <f aca="false">D49/$C49</f>
         <v>1</v>
@@ -4800,14 +5027,14 @@
       <c r="I50" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="J50" s="11" t="n">
+      <c r="J50" s="8" t="n">
         <v>0.314525462962963</v>
       </c>
-      <c r="K50" s="11" t="n">
+      <c r="K50" s="8" t="n">
         <v>0.314560185185185</v>
       </c>
-      <c r="L50" s="11"/>
-      <c r="M50" s="10" t="n">
+      <c r="L50" s="8"/>
+      <c r="M50" s="9" t="n">
         <f aca="false">K50-J50</f>
         <v>3.47222222222222E-005</v>
       </c>
@@ -4862,14 +5089,14 @@
       <c r="I51" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="J51" s="11" t="n">
+      <c r="J51" s="8" t="n">
         <v>0.314583333333333</v>
       </c>
-      <c r="K51" s="11" t="n">
+      <c r="K51" s="8" t="n">
         <v>0.314583333333333</v>
       </c>
-      <c r="L51" s="11"/>
-      <c r="M51" s="10" t="n">
+      <c r="L51" s="8"/>
+      <c r="M51" s="9" t="n">
         <f aca="false">K51-J51</f>
         <v>0</v>
       </c>
@@ -4915,23 +5142,23 @@
       <c r="F52" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G52" s="12" t="n">
+      <c r="G52" s="10" t="n">
         <v>26</v>
       </c>
-      <c r="H52" s="12" t="n">
+      <c r="H52" s="10" t="n">
         <v>30</v>
       </c>
       <c r="I52" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="J52" s="11" t="n">
+      <c r="J52" s="8" t="n">
         <v>0.391168981481482</v>
       </c>
-      <c r="K52" s="11" t="n">
+      <c r="K52" s="8" t="n">
         <v>0.400787037037037</v>
       </c>
-      <c r="L52" s="11"/>
-      <c r="M52" s="10" t="n">
+      <c r="L52" s="8"/>
+      <c r="M52" s="9" t="n">
         <f aca="false">K52-J52</f>
         <v>0.00961805555555556</v>
       </c>
@@ -4989,18 +5216,18 @@
       <c r="I53" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="J53" s="11" t="n">
+      <c r="J53" s="8" t="n">
         <v>0.326851851851852</v>
       </c>
-      <c r="K53" s="11" t="n">
+      <c r="K53" s="8" t="n">
         <v>0.336446759259259</v>
       </c>
-      <c r="L53" s="11"/>
-      <c r="M53" s="10" t="n">
+      <c r="L53" s="8"/>
+      <c r="M53" s="9" t="n">
         <f aca="false">K53-J53</f>
         <v>0.00959490740740741</v>
       </c>
-      <c r="N53" s="11" t="n">
+      <c r="N53" s="8" t="n">
         <v>0.439861111111111</v>
       </c>
       <c r="P53" s="1" t="n">
@@ -5054,14 +5281,14 @@
       <c r="I54" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="J54" s="11" t="n">
+      <c r="J54" s="8" t="n">
         <v>0.476678240740741</v>
       </c>
-      <c r="K54" s="11" t="n">
+      <c r="K54" s="8" t="n">
         <v>0.476701388888889</v>
       </c>
-      <c r="L54" s="11"/>
-      <c r="M54" s="10" t="n">
+      <c r="L54" s="8"/>
+      <c r="M54" s="9" t="n">
         <f aca="false">K54-J54</f>
         <v>2.31481481481481E-005</v>
       </c>
@@ -5116,14 +5343,14 @@
       <c r="I55" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="J55" s="11" t="n">
+      <c r="J55" s="8" t="n">
         <v>0.476840277777778</v>
       </c>
-      <c r="K55" s="11" t="n">
+      <c r="K55" s="8" t="n">
         <v>0.478958333333333</v>
       </c>
-      <c r="L55" s="11"/>
-      <c r="M55" s="10" t="n">
+      <c r="L55" s="8"/>
+      <c r="M55" s="9" t="n">
         <f aca="false">K55-J55</f>
         <v>0.00211805555555556</v>
       </c>
@@ -5178,14 +5405,14 @@
       <c r="I56" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="J56" s="11" t="n">
+      <c r="J56" s="8" t="n">
         <v>0.390173611111111</v>
       </c>
-      <c r="K56" s="11" t="n">
+      <c r="K56" s="8" t="n">
         <v>0.39037037037037</v>
       </c>
-      <c r="L56" s="11"/>
-      <c r="M56" s="10" t="n">
+      <c r="L56" s="8"/>
+      <c r="M56" s="9" t="n">
         <f aca="false">K56-J56</f>
         <v>0.000196759259259259</v>
       </c>
@@ -5226,11 +5453,11 @@
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="10"/>
-      <c r="N57" s="11" t="s">
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="8" t="s">
         <v>34</v>
       </c>
       <c r="P57" s="1" t="e">
@@ -5281,19 +5508,19 @@
       <c r="H58" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="I58" s="8"/>
-      <c r="J58" s="11" t="n">
+      <c r="I58" s="7"/>
+      <c r="J58" s="8" t="n">
         <v>0.459027777777778</v>
       </c>
-      <c r="K58" s="11" t="n">
+      <c r="K58" s="8" t="n">
         <v>0.459027777777778</v>
       </c>
-      <c r="L58" s="11"/>
-      <c r="M58" s="10" t="n">
+      <c r="L58" s="8"/>
+      <c r="M58" s="9" t="n">
         <f aca="false">K58-J58</f>
         <v>0</v>
       </c>
-      <c r="N58" s="11" t="n">
+      <c r="N58" s="8" t="n">
         <v>0.570798611111111</v>
       </c>
       <c r="P58" s="1" t="n">
@@ -5412,1328 +5639,1328 @@
   </sheetPr>
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E89" activeCellId="0" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="5" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="5" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="13" t="n">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="n">
+      <c r="C5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="5" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="13" t="n">
+      <c r="B6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="5" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="11" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="5" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="0" t="n">
+      <c r="A12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="5" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="B13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="5" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="0" t="n">
+      <c r="B14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="5" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="0" t="n">
+      <c r="B15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="5" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="B17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="5" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="5" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="0" t="n">
+      <c r="A20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="0" t="n">
+      <c r="C20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="5" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="0" t="n">
+      <c r="B21" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="5" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="0" t="n">
+      <c r="B22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="5" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="0" t="s">
+      <c r="B25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="5" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="5" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="0" t="n">
+      <c r="A28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="5" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" s="0" t="n">
+      <c r="B29" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="5" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="5" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C31" s="0" t="n">
+      <c r="B31" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="5" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="B33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="5" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="5" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="0" t="n">
+      <c r="A36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="5" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C37" s="0" t="n">
+      <c r="B37" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="5" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" s="0" t="n">
+      <c r="B38" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="5" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="0" t="n">
+      <c r="B39" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="5" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="0" t="s">
+      <c r="B41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="5" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="E43" s="0" t="n">
+      <c r="E43" s="5" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="0" t="n">
+      <c r="A44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="C44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" s="0" t="n">
+      <c r="C44" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C45" s="0" t="n">
+      <c r="B45" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="D45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="0" t="n">
+      <c r="D45" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" s="0" t="n">
+      <c r="B46" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="0" t="n">
+      <c r="B47" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="5" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="0" t="s">
+      <c r="B49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="C50" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="D50" s="0" t="n">
+      <c r="D50" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="E50" s="0" t="n">
+      <c r="E50" s="5" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="C51" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="D51" s="0" t="n">
+      <c r="D51" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51" s="5" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="0" t="n">
+      <c r="A52" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="C52" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="D52" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="E52" s="0" t="n">
+      <c r="E52" s="5" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" s="0" t="n">
+      <c r="B53" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="D53" s="0" t="n">
+      <c r="D53" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="5" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" s="0" t="n">
+      <c r="B54" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="E54" s="0" t="n">
+      <c r="E54" s="5" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B55" s="0" t="n">
+      <c r="B55" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="E55" s="0" t="n">
+      <c r="E55" s="5" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="0" t="s">
+      <c r="B57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="C58" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E58" s="0" t="n">
+      <c r="E58" s="5" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C59" s="0" t="n">
+      <c r="C59" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D59" s="0" t="n">
+      <c r="D59" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E59" s="0" t="n">
+      <c r="E59" s="5" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="0" t="n">
+      <c r="A60" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C60" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" s="0" t="n">
+      <c r="C60" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="E60" s="0" t="n">
+      <c r="E60" s="5" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C61" s="0" t="n">
+      <c r="B61" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D61" s="0" t="n">
+      <c r="D61" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="E61" s="0" t="n">
+      <c r="E61" s="5" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="0" t="n">
+      <c r="B62" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="C62" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D62" s="0" t="n">
+      <c r="D62" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E62" s="0" t="n">
+      <c r="E62" s="5" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C63" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D63" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E63" s="5" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="0" t="s">
+      <c r="B65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="0" t="s">
+      <c r="E65" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B66" s="0" t="n">
+      <c r="B66" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C66" s="5" t="n">
         <v>43</v>
       </c>
-      <c r="D66" s="0" t="n">
+      <c r="D66" s="5" t="n">
         <v>153</v>
       </c>
-      <c r="E66" s="0" t="n">
+      <c r="E66" s="5" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="C67" s="0" t="n">
+      <c r="C67" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D67" s="5" t="n">
         <v>54</v>
       </c>
-      <c r="E67" s="0" t="n">
+      <c r="E67" s="5" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="0" t="n">
+      <c r="A68" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="C68" s="0" t="n">
+      <c r="C68" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="D68" s="0" t="n">
+      <c r="D68" s="5" t="n">
         <v>95</v>
       </c>
-      <c r="E68" s="0" t="n">
+      <c r="E68" s="5" t="n">
         <v>47</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C69" s="0" t="n">
+      <c r="B69" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C69" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D69" s="5" t="n">
         <v>95</v>
       </c>
-      <c r="E69" s="0" t="n">
+      <c r="E69" s="5" t="n">
         <v>37</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C70" s="0" t="n">
+      <c r="C70" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="D70" s="0" t="n">
+      <c r="D70" s="5" t="n">
         <v>159</v>
       </c>
-      <c r="E70" s="0" t="n">
+      <c r="E70" s="5" t="n">
         <v>51</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B71" s="0" t="n">
+      <c r="B71" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C71" s="0" t="n">
+      <c r="C71" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="D71" s="0" t="n">
+      <c r="D71" s="5" t="n">
         <v>48</v>
       </c>
-      <c r="E71" s="0" t="n">
+      <c r="E71" s="5" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" s="0" t="s">
+      <c r="B73" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E73" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="0" t="n">
+      <c r="B74" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="C74" s="0" t="n">
+      <c r="C74" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="D74" s="0" t="n">
+      <c r="D74" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="E74" s="0" t="n">
+      <c r="E74" s="5" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="0" t="n">
+      <c r="B75" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="C75" s="0" t="n">
+      <c r="C75" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="D75" s="0" t="n">
+      <c r="D75" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="E75" s="0" t="n">
+      <c r="E75" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B76" s="0" t="n">
+      <c r="A76" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="C76" s="0" t="n">
+      <c r="C76" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="D76" s="0" t="n">
+      <c r="D76" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="E76" s="0" t="n">
+      <c r="E76" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C77" s="0" t="n">
+      <c r="B77" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C77" s="5" t="n">
         <v>52</v>
       </c>
-      <c r="D77" s="0" t="n">
+      <c r="D77" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="E77" s="0" t="n">
+      <c r="E77" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B78" s="0" t="n">
+      <c r="B78" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="C78" s="0" t="n">
+      <c r="C78" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="D78" s="0" t="n">
+      <c r="D78" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="E78" s="0" t="n">
+      <c r="E78" s="5" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="0" t="n">
+      <c r="B79" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="5" t="n">
         <v>48</v>
       </c>
-      <c r="D79" s="0" t="n">
+      <c r="D79" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="E79" s="0" t="n">
+      <c r="E79" s="5" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="0" t="s">
+      <c r="B81" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="D81" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E81" s="0" t="s">
+      <c r="E81" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B82" s="0" t="n">
+      <c r="B82" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="C82" s="0" t="n">
+      <c r="C82" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="D82" s="0" t="n">
+      <c r="D82" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="E82" s="0" t="n">
+      <c r="E82" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="0" t="n">
+      <c r="B83" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="C83" s="0" t="n">
+      <c r="C83" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="D83" s="0" t="n">
+      <c r="D83" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="E83" s="0" t="n">
+      <c r="E83" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B84" s="0" t="n">
+      <c r="A84" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="C84" s="0" t="n">
+      <c r="C84" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="D84" s="0" t="n">
+      <c r="D84" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E84" s="0" t="n">
+      <c r="E84" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C85" s="0" t="n">
+      <c r="B85" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C85" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="D85" s="0" t="n">
+      <c r="D85" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E85" s="0" t="n">
+      <c r="E85" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B86" s="0" t="n">
+      <c r="B86" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C86" s="0" t="n">
+      <c r="C86" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D86" s="0" t="n">
+      <c r="D86" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="E86" s="0" t="n">
+      <c r="E86" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B87" s="0" t="n">
+      <c r="B87" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="C87" s="0" t="n">
+      <c r="C87" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="D87" s="0" t="n">
+      <c r="D87" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="E87" s="0" t="n">
+      <c r="E87" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E89" s="0" t="n">
+      <c r="E89" s="5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -6747,4 +6974,591 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R29" activeCellId="0" sqref="R29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <v>0.784710648148148</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>0.791805555555556</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>0.798680555555556</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>0.805543981481481</v>
+      </c>
+      <c r="H3" s="12" t="n">
+        <f aca="false">E3-D3</f>
+        <v>0.00709490740740741</v>
+      </c>
+      <c r="I3" s="12" t="n">
+        <f aca="false">F3-E3</f>
+        <v>0.006875</v>
+      </c>
+      <c r="J3" s="12" t="n">
+        <f aca="false">G3-F3</f>
+        <v>0.00686342592592593</v>
+      </c>
+      <c r="K3" s="9" t="n">
+        <f aca="false">G3-D3</f>
+        <v>0.0208333333333333</v>
+      </c>
+      <c r="L3" s="8" t="n">
+        <v>0.428634259259259</v>
+      </c>
+      <c r="M3" s="8" t="n">
+        <v>0.431782407407407</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="9" t="n">
+        <f aca="false">M3-L3</f>
+        <v>0.00314814814814815</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0.759456018518519</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0.759907407407407</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>0.760428240740741</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>0.7609375</v>
+      </c>
+      <c r="H4" s="12" t="n">
+        <f aca="false">E4-D4</f>
+        <v>0.000451388888888889</v>
+      </c>
+      <c r="I4" s="12" t="n">
+        <f aca="false">F4-E4</f>
+        <v>0.000520833333333333</v>
+      </c>
+      <c r="J4" s="12" t="n">
+        <f aca="false">G4-F4</f>
+        <v>0.000509259259259259</v>
+      </c>
+      <c r="K4" s="9" t="n">
+        <f aca="false">G4-D4</f>
+        <v>0.00148148148148148</v>
+      </c>
+      <c r="L4" s="8" t="n">
+        <v>0.387951388888889</v>
+      </c>
+      <c r="M4" s="8" t="n">
+        <v>0.387974537037037</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="9" t="n">
+        <f aca="false">M4-L4</f>
+        <v>2.31481481481481E-005</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>0.760972222222222</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0.761226851851852</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>0.761238425925926</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>0.761238425925926</v>
+      </c>
+      <c r="H5" s="12" t="n">
+        <f aca="false">E5-D5</f>
+        <v>0.00025462962962963</v>
+      </c>
+      <c r="I5" s="12" t="n">
+        <f aca="false">F5-E5</f>
+        <v>1.15740740740741E-005</v>
+      </c>
+      <c r="J5" s="12" t="n">
+        <f aca="false">G5-F5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="9" t="n">
+        <f aca="false">G5-D5</f>
+        <v>0.000266203703703704</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <v>0.314571759259259</v>
+      </c>
+      <c r="M5" s="8" t="n">
+        <v>0.314571759259259</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="9" t="n">
+        <f aca="false">M5-L5</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="15" t="n">
+        <v>0.761296296296296</v>
+      </c>
+      <c r="E6" s="15" t="n">
+        <v>0.768333333333333</v>
+      </c>
+      <c r="F6" s="15" t="n">
+        <v>0.775023148148148</v>
+      </c>
+      <c r="G6" s="15" t="n">
+        <v>0.781712962962963</v>
+      </c>
+      <c r="H6" s="16" t="n">
+        <f aca="false">E6-D6</f>
+        <v>0.00703703703703704</v>
+      </c>
+      <c r="I6" s="16" t="n">
+        <f aca="false">F6-E6</f>
+        <v>0.00668981481481482</v>
+      </c>
+      <c r="J6" s="16" t="n">
+        <f aca="false">G6-F6</f>
+        <v>0.00668981481481482</v>
+      </c>
+      <c r="K6" s="17" t="n">
+        <f aca="false">E6-D6</f>
+        <v>0.00703703703703704</v>
+      </c>
+      <c r="L6" s="15" t="n">
+        <v>0.729328703703704</v>
+      </c>
+      <c r="M6" s="15" t="n">
+        <v>0.755405092592593</v>
+      </c>
+      <c r="N6" s="15" t="n">
+        <v>0.202083333333333</v>
+      </c>
+      <c r="P6" s="17" t="n">
+        <f aca="false">M6-L6</f>
+        <v>0.0260763888888889</v>
+      </c>
+      <c r="Q6" s="17" t="n">
+        <f aca="false">N6-L6+1</f>
+        <v>0.47275462962963</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="19" t="n">
+        <v>0.430011574074074</v>
+      </c>
+      <c r="E7" s="19" t="n">
+        <v>0.467696759259259</v>
+      </c>
+      <c r="F7" s="19" t="n">
+        <v>0.515763888888889</v>
+      </c>
+      <c r="G7" s="19" t="n">
+        <v>0.563680555555556</v>
+      </c>
+      <c r="H7" s="20" t="n">
+        <f aca="false">E7-D7</f>
+        <v>0.0376851851851852</v>
+      </c>
+      <c r="I7" s="20" t="n">
+        <f aca="false">F7-E7</f>
+        <v>0.0480671296296296</v>
+      </c>
+      <c r="J7" s="20" t="n">
+        <f aca="false">G7-F7</f>
+        <v>0.0479166666666667</v>
+      </c>
+      <c r="K7" s="21" t="n">
+        <f aca="false">E7-D7</f>
+        <v>0.0376851851851852</v>
+      </c>
+      <c r="L7" s="19" t="n">
+        <v>0.729768518518519</v>
+      </c>
+      <c r="M7" s="19" t="n">
+        <v>0.73880787037037</v>
+      </c>
+      <c r="N7" s="19" t="n">
+        <v>0.202106481481481</v>
+      </c>
+      <c r="P7" s="21" t="n">
+        <f aca="false">M7-L7</f>
+        <v>0.00903935185185185</v>
+      </c>
+      <c r="Q7" s="22" t="n">
+        <f aca="false">N7-L7+1</f>
+        <v>0.472337962962963</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0.563923611111111</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>0.569305555555556</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>0.569305555555556</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>0.569305555555556</v>
+      </c>
+      <c r="H8" s="12" t="n">
+        <f aca="false">E8-D8</f>
+        <v>0.00538194444444444</v>
+      </c>
+      <c r="I8" s="12" t="n">
+        <f aca="false">F8-E8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="12" t="n">
+        <f aca="false">G8-F8</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="9" t="n">
+        <f aca="false">E8-D8</f>
+        <v>0.00538194444444444</v>
+      </c>
+      <c r="L8" s="8" t="n">
+        <v>0.476678240740741</v>
+      </c>
+      <c r="M8" s="8" t="n">
+        <v>0.476701388888889</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="9" t="n">
+        <f aca="false">M8-L8</f>
+        <v>2.31481481481481E-005</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="19" t="n">
+        <v>0.493101851851852</v>
+      </c>
+      <c r="E9" s="19" t="n">
+        <v>0.49349537037037</v>
+      </c>
+      <c r="F9" s="19" t="n">
+        <v>0.493587962962963</v>
+      </c>
+      <c r="G9" s="19" t="n">
+        <v>0.493680555555556</v>
+      </c>
+      <c r="H9" s="20" t="n">
+        <f aca="false">E9-D9</f>
+        <v>0.000393518518518519</v>
+      </c>
+      <c r="I9" s="20" t="n">
+        <f aca="false">F9-E9</f>
+        <v>9.25925925925926E-005</v>
+      </c>
+      <c r="J9" s="20" t="n">
+        <f aca="false">G9-F9</f>
+        <v>9.25925925925926E-005</v>
+      </c>
+      <c r="K9" s="21" t="n">
+        <f aca="false">E9-D9</f>
+        <v>0.000393518518518519</v>
+      </c>
+      <c r="L9" s="19" t="n">
+        <v>0.730023148148148</v>
+      </c>
+      <c r="M9" s="19" t="n">
+        <v>0.0177777777777778</v>
+      </c>
+      <c r="N9" s="19" t="n">
+        <v>0.202083333333333</v>
+      </c>
+      <c r="P9" s="21" t="n">
+        <f aca="false">M9-L9+1</f>
+        <v>0.28775462962963</v>
+      </c>
+      <c r="Q9" s="21" t="n">
+        <f aca="false">N9-L9+1</f>
+        <v>0.472060185185185</v>
+      </c>
+      <c r="S9" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="19" t="n">
+        <v>0.483981481481481</v>
+      </c>
+      <c r="E10" s="19" t="n">
+        <v>0.488599537037037</v>
+      </c>
+      <c r="F10" s="19" t="n">
+        <v>0.490208333333333</v>
+      </c>
+      <c r="G10" s="19" t="n">
+        <v>0.491805555555556</v>
+      </c>
+      <c r="H10" s="20" t="n">
+        <f aca="false">E10-D10</f>
+        <v>0.00461805555555556</v>
+      </c>
+      <c r="I10" s="20" t="n">
+        <f aca="false">F10-E10</f>
+        <v>0.0016087962962963</v>
+      </c>
+      <c r="J10" s="20" t="n">
+        <f aca="false">G10-F10</f>
+        <v>0.00159722222222222</v>
+      </c>
+      <c r="K10" s="21" t="n">
+        <f aca="false">E10-D10</f>
+        <v>0.00461805555555556</v>
+      </c>
+      <c r="L10" s="19" t="n">
+        <v>0.730173611111111</v>
+      </c>
+      <c r="M10" s="19" t="n">
+        <v>0.730636574074074</v>
+      </c>
+      <c r="N10" s="19" t="n">
+        <v>0.202083333333333</v>
+      </c>
+      <c r="P10" s="21" t="n">
+        <f aca="false">M10-L10</f>
+        <v>0.000462962962962963</v>
+      </c>
+      <c r="Q10" s="21" t="n">
+        <f aca="false">N10-L10+1</f>
+        <v>0.471909722222222</v>
+      </c>
+      <c r="S10" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>0.526006944444444</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>0.635891203703704</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="O13" s="9"/>
+      <c r="P13" s="23" t="n">
+        <f aca="false">M13-L13+1</f>
+        <v>1.10988425925926</v>
+      </c>
+      <c r="Q13" s="9"/>
+      <c r="S13" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>0.446863425925926</v>
+      </c>
+      <c r="M14" s="24" t="n">
+        <v>0.901886574074074</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>0.341550925925926</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="P14" s="23" t="n">
+        <f aca="false">M14-L14</f>
+        <v>0.455023148148148</v>
+      </c>
+      <c r="Q14" s="9" t="n">
+        <f aca="false">N14-L14+1</f>
+        <v>0.8946875</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>0.636412037037037</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.64806712962963</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="O15" s="8"/>
+      <c r="P15" s="12" t="n">
+        <f aca="false">M15-L15</f>
+        <v>0.0116550925925926</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="L1:P1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>